<commit_message>
I have write logger message for in evolution time.
</commit_message>
<xml_diff>
--- a/API_Assignment/Resources/Products.xlsx
+++ b/API_Assignment/Resources/Products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rkunchala/pythonAssignments/Python_Assignments/API_Assignment/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0962590C-9580-FB42-BF6F-C67CEB5CDD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B60DA4-3060-244E-A66F-FA0EA37CBE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{D437161E-1968-C04E-A9C0-77CBFA0C0F5B}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>category</t>
   </si>
   <si>
-    <t>test product</t>
-  </si>
-  <si>
     <t>This is description</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>test product4</t>
+  </si>
+  <si>
+    <t>test product5</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -485,87 +485,87 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3">
         <v>13.5</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3">
         <v>14.5</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>15.5</v>
       </c>
       <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3">
         <v>16.5</v>
       </c>
       <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3">
         <v>17.5</v>
       </c>
       <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>